<commit_message>
Eric added votes 2017
</commit_message>
<xml_diff>
--- a/data/work-in-progress/base_ife_eric_mar2021-excerpt-work.xlsx
+++ b/data/work-in-progress/base_ife_eric_mar2021-excerpt-work.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="114">
   <si>
     <t xml:space="preserve">ord</t>
   </si>
@@ -697,45 +697,44 @@
   <dimension ref="A1:HG1002"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F129" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
-      <selection pane="bottomRight" activeCell="A107" activeCellId="0" sqref="A107"/>
+      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
+      <selection pane="bottomRight" activeCell="B137" activeCellId="0" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="5.12755102040816"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="3" width="0"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="3" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="3" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="4" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="4" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="4" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="4" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="4" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="215" min="31" style="5" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="216" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="3" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="3" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="4" width="6.75"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="4" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="4" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="4" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="4" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="5" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="215" min="31" style="5" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3122,12 +3121,15 @@
       <c r="O25" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P25" s="0"/>
+      <c r="Q25" s="0"/>
       <c r="R25" s="3" t="n">
         <v>1</v>
       </c>
       <c r="S25" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="T25" s="0"/>
       <c r="U25" s="3" t="n">
         <v>1</v>
       </c>
@@ -3140,6 +3142,7 @@
       <c r="AB25" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AC25" s="0"/>
       <c r="AD25" s="5" t="s">
         <v>58</v>
       </c>
@@ -3190,12 +3193,15 @@
       <c r="O26" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P26" s="0"/>
+      <c r="Q26" s="0"/>
       <c r="R26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="S26" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="T26" s="0"/>
       <c r="U26" s="3" t="n">
         <v>1</v>
       </c>
@@ -3208,6 +3214,7 @@
       <c r="AB26" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AC26" s="0"/>
       <c r="AD26" s="5" t="s">
         <v>59</v>
       </c>
@@ -3258,12 +3265,15 @@
       <c r="O27" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P27" s="0"/>
+      <c r="Q27" s="0"/>
       <c r="R27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="S27" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="T27" s="0"/>
       <c r="U27" s="3" t="n">
         <v>1</v>
       </c>
@@ -3276,6 +3286,7 @@
       <c r="AB27" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AC27" s="0"/>
       <c r="AD27" s="5" t="s">
         <v>60</v>
       </c>
@@ -3326,12 +3337,15 @@
       <c r="O28" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P28" s="0"/>
+      <c r="Q28" s="0"/>
       <c r="R28" s="3" t="n">
         <v>2</v>
       </c>
       <c r="S28" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="T28" s="0"/>
       <c r="U28" s="3" t="n">
         <v>1</v>
       </c>
@@ -3344,6 +3358,7 @@
       <c r="AB28" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AC28" s="0"/>
       <c r="AD28" s="5" t="s">
         <v>61</v>
       </c>
@@ -3394,12 +3409,15 @@
       <c r="O29" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P29" s="0"/>
+      <c r="Q29" s="0"/>
       <c r="R29" s="3" t="n">
         <v>2</v>
       </c>
       <c r="S29" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="T29" s="0"/>
       <c r="U29" s="3" t="n">
         <v>1</v>
       </c>
@@ -3412,6 +3430,7 @@
       <c r="AB29" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AC29" s="0"/>
       <c r="AD29" s="5" t="s">
         <v>62</v>
       </c>
@@ -3462,12 +3481,15 @@
       <c r="O30" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P30" s="0"/>
+      <c r="Q30" s="0"/>
       <c r="R30" s="3" t="n">
         <v>1</v>
       </c>
       <c r="S30" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="T30" s="0"/>
       <c r="U30" s="3" t="n">
         <v>1</v>
       </c>
@@ -3480,6 +3502,7 @@
       <c r="AB30" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AC30" s="0"/>
       <c r="AD30" s="5" t="s">
         <v>63</v>
       </c>
@@ -3530,12 +3553,15 @@
       <c r="O31" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P31" s="0"/>
+      <c r="Q31" s="0"/>
       <c r="R31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="S31" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="T31" s="0"/>
       <c r="U31" s="3" t="n">
         <v>1</v>
       </c>
@@ -3548,6 +3574,7 @@
       <c r="AB31" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="AC31" s="0"/>
       <c r="AD31" s="5" t="s">
         <v>64</v>
       </c>
@@ -3572,8 +3599,11 @@
       <c r="M32" s="0"/>
       <c r="N32" s="0"/>
       <c r="O32" s="0"/>
+      <c r="P32" s="0"/>
+      <c r="Q32" s="0"/>
       <c r="R32" s="0"/>
       <c r="S32" s="0"/>
+      <c r="T32" s="0"/>
       <c r="U32" s="0"/>
       <c r="V32" s="0"/>
       <c r="W32" s="0"/>
@@ -3631,12 +3661,15 @@
       <c r="O33" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P33" s="0"/>
+      <c r="Q33" s="0"/>
       <c r="R33" s="3" t="n">
         <v>1</v>
       </c>
       <c r="S33" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="T33" s="0"/>
       <c r="U33" s="3" t="n">
         <v>1</v>
       </c>
@@ -3699,12 +3732,15 @@
       <c r="O34" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P34" s="0"/>
+      <c r="Q34" s="0"/>
       <c r="R34" s="3" t="n">
         <v>1</v>
       </c>
       <c r="S34" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="T34" s="0"/>
       <c r="U34" s="3" t="n">
         <v>1</v>
       </c>
@@ -3725,9 +3761,28 @@
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
       <c r="F35" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
+      <c r="N35" s="0"/>
+      <c r="O35" s="0"/>
+      <c r="P35" s="0"/>
+      <c r="Q35" s="0"/>
+      <c r="R35" s="0"/>
+      <c r="S35" s="0"/>
+      <c r="T35" s="0"/>
+      <c r="AB35" s="0"/>
       <c r="AD35" s="5" t="s">
         <v>33</v>
       </c>
@@ -7057,6 +7112,9 @@
       <c r="T84" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB84" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD84" s="5" t="s">
         <v>33</v>
       </c>
@@ -7122,6 +7180,9 @@
       <c r="T85" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB85" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD85" s="5" t="s">
         <v>33</v>
       </c>
@@ -7187,6 +7248,9 @@
       <c r="T86" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB86" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD86" s="5" t="s">
         <v>33</v>
       </c>
@@ -7252,6 +7316,9 @@
       <c r="T87" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB87" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD87" s="5" t="s">
         <v>33</v>
       </c>
@@ -7317,6 +7384,9 @@
       <c r="T88" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB88" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD88" s="5" t="s">
         <v>33</v>
       </c>
@@ -7382,6 +7452,9 @@
       <c r="T89" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB89" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD89" s="5" t="s">
         <v>33</v>
       </c>
@@ -7447,6 +7520,9 @@
       <c r="T90" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB90" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD90" s="5" t="s">
         <v>33</v>
       </c>
@@ -7512,6 +7588,9 @@
       <c r="T91" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB91" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD91" s="5" t="s">
         <v>33</v>
       </c>
@@ -7577,6 +7656,9 @@
       <c r="T92" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB92" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD92" s="5" t="s">
         <v>33</v>
       </c>
@@ -7642,6 +7724,9 @@
       <c r="T93" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB93" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD93" s="5" t="s">
         <v>33</v>
       </c>
@@ -7707,6 +7792,9 @@
       <c r="T94" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB94" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD94" s="5" t="s">
         <v>33</v>
       </c>
@@ -7772,6 +7860,9 @@
       <c r="T95" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB95" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD95" s="5" t="s">
         <v>33</v>
       </c>
@@ -7837,6 +7928,9 @@
       <c r="T96" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="AB96" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD96" s="5" t="s">
         <v>33</v>
       </c>
@@ -7902,6 +7996,9 @@
       <c r="T97" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB97" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD97" s="5" t="s">
         <v>33</v>
       </c>
@@ -7967,6 +8064,9 @@
       <c r="T98" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB98" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD98" s="5" t="s">
         <v>33</v>
       </c>
@@ -8032,6 +8132,9 @@
       <c r="T99" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB99" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD99" s="5" t="s">
         <v>33</v>
       </c>
@@ -8097,6 +8200,9 @@
       <c r="T100" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="AB100" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD100" s="5" t="s">
         <v>33</v>
       </c>
@@ -8162,6 +8268,9 @@
       <c r="T101" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB101" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD101" s="5" t="s">
         <v>33</v>
       </c>
@@ -8227,6 +8336,9 @@
       <c r="T102" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB102" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD102" s="5" t="s">
         <v>33</v>
       </c>
@@ -8292,6 +8404,9 @@
       <c r="T103" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB103" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD103" s="5" t="s">
         <v>33</v>
       </c>
@@ -8357,6 +8472,9 @@
       <c r="T104" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB104" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD104" s="5" t="s">
         <v>33</v>
       </c>
@@ -8422,6 +8540,9 @@
       <c r="T105" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB105" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD105" s="5" t="s">
         <v>33</v>
       </c>
@@ -8487,6 +8608,9 @@
       <c r="T106" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="AB106" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD106" s="5" t="s">
         <v>33</v>
       </c>
@@ -8495,8 +8619,65 @@
       <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
+      <c r="B107" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F107" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G107" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q107" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S107" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T107" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB107" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD107" s="5" t="s">
         <v>33</v>
@@ -8506,8 +8687,65 @@
       <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
+      <c r="B108" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F108" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G108" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q108" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S108" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T108" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB108" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD108" s="5" t="s">
         <v>33</v>
@@ -8517,8 +8755,65 @@
       <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
+      <c r="B109" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F109" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G109" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q109" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S109" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T109" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB109" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD109" s="5" t="s">
         <v>33</v>
@@ -8528,8 +8823,65 @@
       <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
+      <c r="B110" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F110" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G110" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q110" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S110" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T110" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB110" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD110" s="5" t="s">
         <v>33</v>
@@ -8539,8 +8891,65 @@
       <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
+      <c r="B111" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C111" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F111" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L111" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T111" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB111" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD111" s="5" t="s">
         <v>33</v>
@@ -8550,8 +8959,65 @@
       <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
+      <c r="B112" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C112" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F112" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L112" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O112" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q112" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S112" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T112" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB112" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD112" s="5" t="s">
         <v>33</v>
@@ -8561,8 +9027,65 @@
       <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
+      <c r="B113" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C113" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F113" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L113" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q113" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S113" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T113" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB113" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD113" s="5" t="s">
         <v>33</v>
@@ -8572,8 +9095,65 @@
       <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
+      <c r="B114" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C114" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F114" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J114" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K114" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L114" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M114" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N114" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O114" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P114" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q114" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R114" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S114" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T114" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB114" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD114" s="5" t="s">
         <v>33</v>
@@ -8583,8 +9163,65 @@
       <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
+      <c r="B115" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C115" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D115" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F115" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I115" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J115" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K115" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L115" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M115" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N115" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O115" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P115" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q115" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R115" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S115" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="T115" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB115" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD115" s="5" t="s">
         <v>33</v>
@@ -8594,8 +9231,65 @@
       <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
+      <c r="B116" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D116" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F116" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I116" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J116" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K116" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L116" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M116" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N116" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O116" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P116" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q116" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R116" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S116" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T116" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB116" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD116" s="5" t="s">
         <v>33</v>
@@ -8605,8 +9299,65 @@
       <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
+      <c r="B117" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F117" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I117" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J117" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K117" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L117" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M117" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N117" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O117" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P117" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q117" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R117" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S117" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T117" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB117" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD117" s="5" t="s">
         <v>33</v>
@@ -8616,8 +9367,65 @@
       <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
+      <c r="B118" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D118" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E118" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F118" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB118" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD118" s="5" t="s">
         <v>33</v>
@@ -8627,8 +9435,65 @@
       <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
+      <c r="B119" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D119" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E119" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F119" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB119" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD119" s="5" t="s">
         <v>33</v>
@@ -8638,8 +9503,65 @@
       <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
+      <c r="B120" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F120" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T120" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB120" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD120" s="5" t="s">
         <v>33</v>
@@ -8649,8 +9571,65 @@
       <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
+      <c r="B121" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="C121" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D121" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F121" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T121" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB121" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD121" s="5" t="s">
         <v>33</v>
@@ -8660,8 +9639,65 @@
       <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
+      <c r="B122" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="C122" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D122" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F122" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T122" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB122" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD122" s="5" t="s">
         <v>33</v>
@@ -8671,8 +9707,65 @@
       <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
+      <c r="B123" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="C123" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D123" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F123" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB123" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD123" s="5" t="s">
         <v>33</v>
@@ -8682,8 +9775,65 @@
       <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
+      <c r="B124" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="C124" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D124" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E124" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F124" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L124" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N124" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q124" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S124" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T124" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB124" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD124" s="5" t="s">
         <v>33</v>
@@ -8693,8 +9843,65 @@
       <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
+      <c r="B125" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="C125" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D125" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E125" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F125" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T125" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB125" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD125" s="5" t="s">
         <v>33</v>
@@ -8704,8 +9911,65 @@
       <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
+      <c r="B126" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="C126" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D126" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F126" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T126" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB126" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD126" s="5" t="s">
         <v>33</v>
@@ -8715,8 +9979,65 @@
       <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
+      <c r="B127" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="C127" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D127" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F127" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB127" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD127" s="5" t="s">
         <v>33</v>
@@ -8726,8 +10047,65 @@
       <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
+      <c r="B128" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="C128" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D128" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F128" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G128" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M128" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O128" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q128" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R128" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S128" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T128" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB128" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD128" s="5" t="s">
         <v>33</v>
@@ -8737,8 +10115,65 @@
       <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
+      <c r="B129" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="C129" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D129" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E129" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F129" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G129" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB129" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD129" s="5" t="s">
         <v>33</v>
@@ -8748,8 +10183,65 @@
       <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
+      <c r="B130" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="C130" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D130" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F130" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I130" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J130" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K130" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L130" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M130" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N130" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O130" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P130" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q130" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R130" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S130" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T130" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB130" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD130" s="5" t="s">
         <v>33</v>
@@ -8759,8 +10251,65 @@
       <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
+      <c r="B131" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D131" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F131" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G131" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q131" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R131" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S131" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="T131" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB131" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD131" s="5" t="s">
         <v>33</v>
@@ -8770,8 +10319,65 @@
       <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
+      <c r="B132" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="C132" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D132" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F132" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G132" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q132" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R132" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="S132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T132" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB132" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD132" s="5" t="s">
         <v>33</v>
@@ -8781,8 +10387,65 @@
       <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
+      <c r="B133" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="C133" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D133" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F133" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G133" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K133" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L133" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M133" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N133" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O133" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P133" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q133" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R133" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S133" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="T133" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB133" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD133" s="5" t="s">
         <v>33</v>
@@ -8792,8 +10455,65 @@
       <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
+      <c r="B134" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="C134" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D134" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F134" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G134" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T134" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB134" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD134" s="5" t="s">
         <v>33</v>
@@ -8803,8 +10523,65 @@
       <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
+      <c r="B135" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D135" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F135" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G135" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T135" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB135" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD135" s="5" t="s">
         <v>33</v>
@@ -8814,8 +10591,65 @@
       <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
+      <c r="B136" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D136" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>2017</v>
+      </c>
       <c r="F136" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G136" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB136" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="AD136" s="5" t="s">
         <v>33</v>
@@ -15248,11 +17082,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="22" customFormat="true" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>